<commit_message>
added charts to results. Currently timing exhaustive searches... shoudl take forever...
@kelsong
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
+    <sheet name="TimedPerformanceData" sheetId="5" r:id="rId2"/>
+    <sheet name="TimedPerformanceChart" sheetId="6" r:id="rId3"/>
+    <sheet name="ComparisonToOptimalData" sheetId="2" r:id="rId4"/>
+    <sheet name="ComparisonToOptimalChart" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>Data Set</t>
   </si>
@@ -158,6 +160,889 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Timed Performance of Algorithms that Found Global</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Solution</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Full Enumeration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimedPerformanceData!$C$3:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Move</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimedPerformanceData!$D$3:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10863</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Walk</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimedPerformanceData!$E$3:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7403</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ant Colony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimedPerformanceData!$F$3:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Walk</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimedPerformanceData!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimedPerformanceData!$G$3:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3715</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="98913280"/>
+        <c:axId val="98935552"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="98913280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98935552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="98935552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="15000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98913280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithm Performance Compared to Optimal Result</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>global8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>global14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>global23</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparisonToOptimalData!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Move</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>global8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>global14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>global23</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparisonToOptimalData!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Walk</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>global8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>global14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>global23</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparisonToOptimalData!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ant Colony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>global8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>global14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>global23</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparisonToOptimalData!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Walk</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ComparisonToOptimalData!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>global3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>global9a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>global9b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>global8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>global14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>global23</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparisonToOptimalData!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="90276224"/>
+        <c:axId val="90277760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90276224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90277760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90277760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90276224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8678333" cy="6297083"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8678333" cy="6297083"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +1387,9 @@
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>108</v>
+      </c>
       <c r="D3" s="1">
         <v>19</v>
       </c>
@@ -643,24 +1530,363 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>108</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1">
+        <v>133</v>
+      </c>
+      <c r="F3" s="2">
+        <v>76</v>
+      </c>
+      <c r="G3" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10863</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7403</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6662</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3715</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>59710</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>10154</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>